<commit_message>
found GSM bounds when constrained with 13C-MFA and plotted the different bounds for central reactions
</commit_message>
<xml_diff>
--- a/data/13c_mfa/Full MFA data 01192024.xlsx
+++ b/data/13c_mfa/Full MFA data 01192024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/garrettroell/yarrowia_eflux2/data/13c_mfa/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C775E294-B5FC-3C43-A052-5E014788D980}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8729D99B-894A-D64D-A030-69D67ABF55E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22960" yWindow="500" windowWidth="28240" windowHeight="25640" xr2:uid="{829D5511-B240-4489-B127-1E1861E10782}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="692" uniqueCount="268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="692" uniqueCount="269">
   <si>
     <t>Pathway</t>
   </si>
@@ -841,6 +841,9 @@
   </si>
   <si>
     <t>biomass_oil</t>
+  </si>
+  <si>
+    <t>biomass_glucose or biomass_oil</t>
   </si>
 </sst>
 </file>
@@ -1291,7 +1294,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC5C5"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1305,7 +1308,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
+          <bgColor rgb="FFFFC5C5"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1347,14 +1350,14 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
+          <bgColor rgb="FFFFC5C5"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC5C5"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1671,7 +1674,7 @@
   <dimension ref="A1:O73"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E38" sqref="E38"/>
+      <selection activeCell="D69" sqref="D69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4663,7 +4666,7 @@
         <v>237</v>
       </c>
       <c r="D69" s="4" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="E69" s="4"/>
       <c r="F69" s="15">
@@ -9729,14 +9732,14 @@
     <mergeCell ref="G1:X1"/>
   </mergeCells>
   <conditionalFormatting sqref="L7:L46 R7:R46 L70:L71 R70:R71 L74 R74">
-    <cfRule type="cellIs" dxfId="12" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="7" operator="equal">
+      <formula>"LB NF"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="11" priority="9" operator="equal">
       <formula>"NF"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="8" operator="equal">
       <formula>"UB NF"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="7" operator="equal">
-      <formula>"LB NF"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L2:X5 L6:W6 M7:Q46 S7:W46 L47:X69 M70:Q71 S70:W71 L72:X73 M74:Q74 S74:W74">
@@ -9756,25 +9759,25 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X6:X46">
-    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
+      <formula>"NF"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
       <formula>"UB NF"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
       <formula>"LB NF"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="6" operator="equal">
-      <formula>"NF"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X70:X71 X74">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
-      <formula>"LB NF"</formula>
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+      <formula>"UB NF"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
       <formula>"NF"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
-      <formula>"UB NF"</formula>
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+      <formula>"LB NF"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>